<commit_message>
Add PDF for datapath
</commit_message>
<xml_diff>
--- a/doc/Instructions.xlsx
+++ b/doc/Instructions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="219">
   <si>
     <t>指令</t>
   </si>
@@ -1356,15 +1356,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="4"/>
     <col min="2" max="2" width="16.125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="40" style="3" customWidth="1"/>
+    <col min="3" max="3" width="48.125" style="3" customWidth="1"/>
     <col min="4" max="4" width="23.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.875" style="3" customWidth="1"/>
     <col min="6" max="6" width="25.625" style="1" customWidth="1"/>
@@ -2218,21 +2218,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="4"/>
     <col min="2" max="2" width="16.125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="3"/>
+    <col min="3" max="3" width="41.75" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2240,13 +2241,16 @@
         <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -2254,13 +2258,16 @@
         <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -2268,13 +2275,16 @@
         <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -2282,29 +2292,38 @@
         <v>32</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="C5" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="C6" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -2312,13 +2331,16 @@
         <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -2326,13 +2348,16 @@
         <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -2340,13 +2365,16 @@
         <v>39</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -2354,13 +2382,16 @@
         <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -2368,29 +2399,38 @@
         <v>59</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="C12" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="C13" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -2398,13 +2438,16 @@
         <v>43</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
@@ -2412,13 +2455,16 @@
         <v>134</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D15" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
@@ -2426,69 +2472,93 @@
         <v>45</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="C17" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="C18" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="C19" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="C20" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="C21" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="C22" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="C23" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="7" t="s">
         <v>21</v>
       </c>
@@ -2496,13 +2566,16 @@
         <v>51</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D24" s="3">
+      <c r="E24" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:5">
       <c r="A25" s="8" t="s">
         <v>28</v>
       </c>
@@ -2510,13 +2583,16 @@
         <v>58</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="8" t="s">
         <v>26</v>
       </c>
@@ -2524,13 +2600,16 @@
         <v>56</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D26" s="3">
+      <c r="E26" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" s="7" t="s">
         <v>22</v>
       </c>
@@ -2538,29 +2617,38 @@
         <v>52</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D27" s="3">
+      <c r="E27" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="C28" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="C29" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="7" t="s">
         <v>24</v>
       </c>
@@ -2568,13 +2656,16 @@
         <v>54</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="D30" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
         <v>25</v>
       </c>
@@ -2582,9 +2673,12 @@
         <v>55</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="3">
+      <c r="E31" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3008,5 +3102,6 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix a bug in controller design
</commit_message>
<xml_diff>
--- a/doc/Instructions.xlsx
+++ b/doc/Instructions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="221">
   <si>
     <t>指令</t>
   </si>
@@ -829,6 +829,14 @@
   </si>
   <si>
     <t>011</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>first5 = "11101" and last5 = "01011"</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>0101</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -1356,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1683,6 +1691,9 @@
       <c r="F12" s="6" t="s">
         <v>100</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="H12" s="1" t="s">
         <v>148</v>
       </c>
@@ -2220,8 +2231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2533,7 +2544,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>88</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="1:5">

</xml_diff>

<commit_message>
Getting Over It With Bennett Foddy
</commit_message>
<xml_diff>
--- a/doc/Instructions.xlsx
+++ b/doc/Instructions.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="220">
   <si>
     <t>指令</t>
   </si>
@@ -620,10 +620,6 @@
   </si>
   <si>
     <t>BranchType(2:0)</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>MemToReg</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
@@ -1365,13 +1361,13 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9" style="4"/>
-    <col min="2" max="2" width="16.125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="19.375" style="5" customWidth="1"/>
     <col min="3" max="3" width="48.125" style="3" customWidth="1"/>
     <col min="4" max="4" width="23.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.875" style="3" customWidth="1"/>
@@ -1379,11 +1375,11 @@
     <col min="7" max="7" width="18.75" style="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1"/>
     <col min="9" max="11" width="9" style="3"/>
-    <col min="13" max="13" width="16.25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.25" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1417,14 +1413,11 @@
       <c r="K1" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:12">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1450,7 +1443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:12">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -1476,7 +1469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:12">
       <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
@@ -1502,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:12">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
@@ -1531,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:12">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -1560,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:12">
       <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
@@ -1576,11 +1569,11 @@
       <c r="H7" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="L7" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -1599,11 +1592,11 @@
       <c r="H8" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="L8" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -1622,11 +1615,11 @@
       <c r="H9" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="L9" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="7" t="s">
         <v>9</v>
       </c>
@@ -1645,11 +1638,11 @@
       <c r="H10" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="L10" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="8" t="s">
         <v>29</v>
       </c>
@@ -1668,11 +1661,11 @@
       <c r="H11" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="L11" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -1692,13 +1685,16 @@
         <v>100</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
@@ -1720,11 +1716,11 @@
       <c r="H13" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="L13" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
@@ -1750,7 +1746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:12">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
@@ -1779,11 +1775,8 @@
       <c r="J15" s="3">
         <v>1</v>
       </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="7" t="s">
         <v>14</v>
       </c>
@@ -1809,9 +1802,6 @@
         <v>1</v>
       </c>
       <c r="J16" s="3">
-        <v>1</v>
-      </c>
-      <c r="L16">
         <v>1</v>
       </c>
     </row>
@@ -2232,7 +2222,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A30" sqref="A30:XFD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2544,7 +2534,7 @@
         <v>57</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2703,8 +2693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2717,13 +2707,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2731,10 +2721,10 @@
         <v>104</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2742,10 +2732,10 @@
         <v>115</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2753,10 +2743,10 @@
         <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2764,10 +2754,10 @@
         <v>113</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2775,10 +2765,10 @@
         <v>123</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2786,10 +2776,10 @@
         <v>106</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2797,10 +2787,10 @@
         <v>122</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2808,10 +2798,10 @@
         <v>118</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2819,10 +2809,10 @@
         <v>105</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2830,10 +2820,10 @@
         <v>145</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2841,7 +2831,7 @@
         <v>141</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2849,15 +2839,15 @@
         <v>119</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2865,7 +2855,7 @@
         <v>120</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2873,7 +2863,7 @@
         <v>126</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2881,7 +2871,7 @@
         <v>108</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2895,7 +2885,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2907,10 +2897,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2918,7 +2908,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2926,7 +2916,7 @@
         <v>115</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2934,7 +2924,7 @@
         <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2942,7 +2932,7 @@
         <v>113</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2950,7 +2940,7 @@
         <v>123</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2958,7 +2948,7 @@
         <v>106</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2966,7 +2956,7 @@
         <v>122</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2974,7 +2964,7 @@
         <v>118</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2982,7 +2972,7 @@
         <v>105</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2990,7 +2980,7 @@
         <v>145</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2998,7 +2988,7 @@
         <v>141</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3006,15 +2996,15 @@
         <v>119</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3022,7 +3012,7 @@
         <v>120</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -3030,7 +3020,7 @@
         <v>126</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -3038,7 +3028,7 @@
         <v>108</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3052,7 +3042,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3064,50 +3054,50 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>